<commit_message>
rewrite model files and complete day041
</commit_message>
<xml_diff>
--- a/SQL-daily-exercises/LeetCode_SQL_difficult.xlsx
+++ b/SQL-daily-exercises/LeetCode_SQL_difficult.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VScode-for-cicero\SQL-exercises\SQL-daily-exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31271C31-AFA8-4286-897A-B58BB20E58F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECB2F55-48DA-4004-8A14-4F56ECA21FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,7 +726,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -942,7 +942,9 @@
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>-1</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -989,7 +991,9 @@
       <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1">
+        <v>-1</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">

</xml_diff>

<commit_message>
coplete day052 with Disabling Copilot
</commit_message>
<xml_diff>
--- a/SQL-daily-exercises/LeetCode_SQL_difficult.xlsx
+++ b/SQL-daily-exercises/LeetCode_SQL_difficult.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VScode-for-cicero\SQL-exercises\SQL-daily-exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAF9977-C44B-4A22-A864-066A7A3D54D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B117509B-3608-4985-AAAE-04AD156D81BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -783,8 +783,8 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -828,11 +828,11 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF($C$3:$C$46,1)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I2" s="4">
         <f>ROUND(H2/G2,2)</f>
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
@@ -1411,7 +1411,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1">
@@ -1459,7 +1459,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1">

</xml_diff>